<commit_message>
Several bug fixes. Monsters get now only 50% dmg bonus to non-AT_WEAP-attaks. Weapon-to-hit is now consistent between u-hit-m, polyu-hit-m, m-hit-u, m-hit-m. Several bug fixes.
</commit_message>
<xml_diff>
--- a/HitAndDamageCases.xlsx
+++ b/HitAndDamageCases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="86">
   <si>
     <t>Melee</t>
   </si>
@@ -47,21 +47,12 @@
     <t>Monster - Normal (hit you)</t>
   </si>
   <si>
-    <t>Monster - Weapon (hit you)</t>
-  </si>
-  <si>
     <t>Monster - Normal (hit monster)</t>
   </si>
   <si>
     <t>Monster - Weapon (hit monster)</t>
   </si>
   <si>
-    <t>find_roll_to_hit has abon()</t>
-  </si>
-  <si>
-    <t>find_roll_to_hit has abon(), called from hitum</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Ammo and launcher</t>
   </si>
   <si>
@@ -86,9 +77,6 @@
     <t>hmon_hitmon gives no bonus</t>
   </si>
   <si>
-    <t>thitmonst had ranged_abon(), get additional point blank minus, add hitval (+X - rustedness etc.) and weapon_hit_bonus (from skill), and bracers bonus, bows get a minus with gauntlets, get hitval(projectile) from omon_adj</t>
-  </si>
-  <si>
     <t>thitmonst had ranged_abon(), -extra 4 to hit, get hitval(projectile) from omon_adj</t>
   </si>
   <si>
@@ -165,6 +153,135 @@
   </si>
   <si>
     <t>AC Damage Randomizer</t>
+  </si>
+  <si>
+    <t>mattacku</t>
+  </si>
+  <si>
+    <t>mattacku() has mabon()</t>
+  </si>
+  <si>
+    <t>YES; ONE RANDOMIZATION FOR ALL ATTACKS!!</t>
+  </si>
+  <si>
+    <t>hitmu</t>
+  </si>
+  <si>
+    <t>mattacku/hitmu</t>
+  </si>
+  <si>
+    <t>mattacku has hitval()</t>
+  </si>
+  <si>
+    <t>find_roll_to_hit has abon(), hitval(), and weapon_hit_bonus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Melee - Weapon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Melee - Claw etc.</t>
+  </si>
+  <si>
+    <t>thrwmu+thitu</t>
+  </si>
+  <si>
+    <t>mattacku/thrwmu/thitu</t>
+  </si>
+  <si>
+    <t>thrwmu+thitu+losehp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Pole "thrown"</t>
+  </si>
+  <si>
+    <t>mattacku/thrwmu/monshoot/m_throw</t>
+  </si>
+  <si>
+    <t>thitmonst had ranged_abon(), get weapon_hit_bonus (skill), get hitval(projectile) from omon_adj, launcher bonus, point blank adjustment</t>
+  </si>
+  <si>
+    <t>mattacku/thrwmu/monshoot/m_throw/thitu</t>
+  </si>
+  <si>
+    <t>m_throw+thitu+losehp</t>
+  </si>
+  <si>
+    <t>m_throw() has mdbon(), dmgval(projectile), dmgval(laucher)</t>
+  </si>
+  <si>
+    <t>thrwmu() has mdbon(), dmgval(pole)</t>
+  </si>
+  <si>
+    <t>m_throw() has 10, m_lev, mrabon(), hitval(projectile), hitval(laucher), distance adjustment, point blank adjustment, bracers missing</t>
+  </si>
+  <si>
+    <t>m_throw() has 10, m_lev, mrabon(), hitval(projectile), -4, distance adjustment</t>
+  </si>
+  <si>
+    <t>thrwmu() has dmgval(projectile)</t>
+  </si>
+  <si>
+    <t>thrwmu() has mdbon(), dmgval(projectile)</t>
+  </si>
+  <si>
+    <t>thrwmu() has 10, m_lev, mrabon(), normal ranged adjustment, hitval(pole)</t>
+  </si>
+  <si>
+    <t>m_throw() has 10, m_lev, mrabon(), normal ranged adjustment, hitval(), point blank adjustment</t>
+  </si>
+  <si>
+    <t>m_throw</t>
+  </si>
+  <si>
+    <t>fightm/mattackm</t>
+  </si>
+  <si>
+    <t>mattacku has AC, m_lev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Thrown weapon</t>
+  </si>
+  <si>
+    <t>mattacku has AC, m_lev, hitval(mw), mabon</t>
+  </si>
+  <si>
+    <t>mattackm</t>
+  </si>
+  <si>
+    <t>mattacku has AC, m_lev, mabon</t>
+  </si>
+  <si>
+    <t>mdamagem</t>
+  </si>
+  <si>
+    <t>fightm/mattackm/hitmm/mdamagem</t>
+  </si>
+  <si>
+    <t>tmp = d((int)mattk-&gt;damn, (int)mattk-&gt;damd) + (int)mattk-&gt;damp + mdbon(magr);</t>
+  </si>
+  <si>
+    <t>fightm/mattackm/thrwmm/monshoot/m_throw</t>
+  </si>
+  <si>
+    <t>NOT USED</t>
+  </si>
+  <si>
+    <t>mattacku has MOD_AC, 10, hitval(weapon)</t>
+  </si>
+  <si>
+    <t>if(mattk-&gt;damn &gt; 0 &amp;&amp; mattk-&gt;damd &gt; 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    dmg += d((int) mattk-&gt;damn, (int) mattk-&gt;damd);</t>
+  </si>
+  <si>
+    <t>dmg += (int)mattk-&gt;damp;</t>
+  </si>
+  <si>
+    <t>mdbon, dmgval</t>
+  </si>
+  <si>
+    <t>Monsters used to do WEAPON + AT_WEAP + STRBONUS damage</t>
   </si>
 </sst>
 </file>
@@ -509,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L20"/>
+  <dimension ref="B1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:I11"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,13 +665,13 @@
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>0</v>
@@ -563,13 +680,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>0</v>
@@ -590,128 +707,128 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
@@ -719,84 +836,84 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -806,30 +923,351 @@
       <c r="B12" t="s">
         <v>6</v>
       </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>7</v>
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" t="s">
+        <v>59</v>
+      </c>
+      <c r="L15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" t="s">
+        <v>54</v>
+      </c>
+      <c r="L16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" t="s">
+        <v>58</v>
+      </c>
+      <c r="J17" t="s">
+        <v>59</v>
+      </c>
+      <c r="L17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" t="s">
+        <v>59</v>
+      </c>
+      <c r="L18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>42</v>
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" t="s">
+        <v>76</v>
+      </c>
+      <c r="J20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" t="s">
+        <v>76</v>
+      </c>
+      <c r="J21" t="s">
+        <v>75</v>
+      </c>
+      <c r="K21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" t="s">
+        <v>58</v>
+      </c>
+      <c r="J22" t="s">
+        <v>59</v>
+      </c>
+      <c r="L22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" t="s">
+        <v>58</v>
+      </c>
+      <c r="J24" t="s">
+        <v>59</v>
+      </c>
+      <c r="L24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" t="s">
+        <v>63</v>
+      </c>
+      <c r="H25" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" t="s">
+        <v>59</v>
+      </c>
+      <c r="L25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J28" t="s">
+        <v>46</v>
+      </c>
+      <c r="L28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weights are now shown in inventory menus and elsewhere
</commit_message>
<xml_diff>
--- a/HitAndDamageCases.xlsx
+++ b/HitAndDamageCases.xlsx
@@ -128,10 +128,10 @@
     <t>attack/hitum</t>
   </si>
   <si>
+    <t>damageum</t>
+  </si>
+  <si>
     <t>hmonas/damageum/</t>
-  </si>
-  <si>
-    <t>damageumon</t>
   </si>
   <si>
     <t>hmonas/known_hitum/hmon/hmon_hitmon</t>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -887,13 +887,13 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" t="s">
         <v>34</v>
-      </c>
-      <c r="I10" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">

</xml_diff>